<commit_message>
analisis de los hubs
</commit_message>
<xml_diff>
--- a/results/stimulated_NAMU_results_analysis/functional_analysis_of_hubs/optimalhubs.xlsx
+++ b/results/stimulated_NAMU_results_analysis/functional_analysis_of_hubs/optimalhubs.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -390,10 +390,20 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>recon3_genes</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Lewis2010_genes</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>VMH_gene_IDs</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>KEGG_genes</t>
         </is>

</xml_diff>